<commit_message>
saved multiply to records
</commit_message>
<xml_diff>
--- a/Instructions/RECORDS.xlsx
+++ b/Instructions/RECORDS.xlsx
@@ -12,10 +12,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CNTR INIT" sheetId="1" r:id="rId1"/>
+    <sheet name="MULTIPLY" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="79">
   <si>
     <t>000000</t>
   </si>
@@ -102,6 +103,168 @@
   </si>
   <si>
     <t>COUNTER INITIALISATION</t>
+  </si>
+  <si>
+    <t>HALT INPUT</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>AND OP</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>A EQL B</t>
+  </si>
+  <si>
+    <t>STEP</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>001010</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>BITSHIFT</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>001100</t>
+  </si>
+  <si>
+    <t>001101</t>
+  </si>
+  <si>
+    <t>001110</t>
+  </si>
+  <si>
+    <t>010000</t>
+  </si>
+  <si>
+    <t>001111</t>
+  </si>
+  <si>
+    <t>010001</t>
+  </si>
+  <si>
+    <t>010010</t>
+  </si>
+  <si>
+    <t>010011</t>
+  </si>
+  <si>
+    <t>010100</t>
+  </si>
+  <si>
+    <t>010101</t>
+  </si>
+  <si>
+    <t>010110</t>
+  </si>
+  <si>
+    <t>010111</t>
+  </si>
+  <si>
+    <t>011001</t>
+  </si>
+  <si>
+    <t>011000</t>
+  </si>
+  <si>
+    <t>011010</t>
+  </si>
+  <si>
+    <t>011011</t>
+  </si>
+  <si>
+    <t>011100</t>
+  </si>
+  <si>
+    <t>011101</t>
+  </si>
+  <si>
+    <t>011110</t>
+  </si>
+  <si>
+    <t>011111</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>100010</t>
+  </si>
+  <si>
+    <t>100001</t>
+  </si>
+  <si>
+    <t>100011</t>
+  </si>
+  <si>
+    <t>100100</t>
+  </si>
+  <si>
+    <t>100101</t>
+  </si>
+  <si>
+    <t>100110</t>
+  </si>
+  <si>
+    <t>100111</t>
+  </si>
+  <si>
+    <t>101000</t>
+  </si>
+  <si>
+    <t>101001</t>
+  </si>
+  <si>
+    <t>101011</t>
+  </si>
+  <si>
+    <t>101010</t>
+  </si>
+  <si>
+    <t>101100</t>
+  </si>
+  <si>
+    <t>101101</t>
+  </si>
+  <si>
+    <t>101110</t>
+  </si>
+  <si>
+    <t>101111</t>
+  </si>
+  <si>
+    <t>110000</t>
+  </si>
+  <si>
+    <t>110001</t>
+  </si>
+  <si>
+    <t>110010</t>
+  </si>
+  <si>
+    <t>110100</t>
+  </si>
+  <si>
+    <t>110011</t>
   </si>
 </sst>
 </file>
@@ -207,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -226,6 +389,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -808,4 +974,1424 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H48" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H50" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H54" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[Binary Instructions.xlsx]HEX GEN BACKEND'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>D54 F54 H54</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[Binary Instructions.xlsx]HEX GEN BACKEND'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F53 H2:H53 D2:D53</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[Binary Instructions.xlsx]HEX GEN BACKEND'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B54</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
A SQUARE B COMPLETE
</commit_message>
<xml_diff>
--- a/Instructions/RECORDS.xlsx
+++ b/Instructions/RECORDS.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CNTR INIT" sheetId="1" r:id="rId1"/>
-    <sheet name="MULTIPLY 2" sheetId="3" r:id="rId2"/>
-    <sheet name="MULTIPLY 3" sheetId="4" r:id="rId3"/>
+    <sheet name="MULTIPLY 3" sheetId="4" r:id="rId2"/>
+    <sheet name="MULTIPLY 2" sheetId="3" r:id="rId3"/>
     <sheet name="MULTIPLY" sheetId="2" r:id="rId4"/>
+    <sheet name="A SQUARE PLUS B SQUARE" sheetId="5" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="84">
   <si>
     <t>000000</t>
   </si>
@@ -279,6 +280,9 @@
   </si>
   <si>
     <t>C5</t>
+  </si>
+  <si>
+    <t>A3</t>
   </si>
 </sst>
 </file>
@@ -301,7 +305,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,6 +327,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -391,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -411,6 +421,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -420,13 +437,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -740,16 +753,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="21"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1012,6 +1025,568 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[Binary Instructions.xlsx]HEX GEN BACKEND'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>D21 F21 H21 D19 F19 H19</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[Binary Instructions.xlsx]HEX GEN BACKEND'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F18 D2:D18 H2:H18 F20 D20 H20</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[Binary Instructions.xlsx]HEX GEN BACKEND'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B21</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H23"/>
   <sheetViews>
@@ -1625,568 +2200,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="28" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="28" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="H8" s="28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="H9" s="28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="28" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="H17" s="28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="F19" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="H19" s="28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="H20" s="28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="G21" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="H21" s="28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'[Binary Instructions.xlsx]HEX GEN BACKEND'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D21 F21 H21 D19 F19 H19</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'[Binary Instructions.xlsx]HEX GEN BACKEND'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F18 D2:D18 H2:H18 F20 D20 H20</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'[Binary Instructions.xlsx]HEX GEN BACKEND'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B21</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H54"/>
@@ -3605,4 +3618,1008 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="H25" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G32" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G33" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H34" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="H35" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F37" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H37" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G38" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[Binary Instructions.xlsx]HEX GEN BACKEND'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>D21 H21 F21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[Binary Instructions.xlsx]HEX GEN BACKEND'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F20 D2:D20 H2:H20 F22:F38 D22:D38 H22:H38</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[Binary Instructions.xlsx]HEX GEN BACKEND'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B38</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>